<commit_message>
schedule for cs major outputted
</commit_message>
<xml_diff>
--- a/class_schedules_fall_2018/COMPUTER SCIENCE (CSCI).xlsx
+++ b/class_schedules_fall_2018/COMPUTER SCIENCE (CSCI).xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="17940" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -343,9 +348,6 @@
     <t>Human Computer Interface</t>
   </si>
   <si>
-    <t>Computer &amp; Inform. Security</t>
-  </si>
-  <si>
     <t>Theory of Computation</t>
   </si>
   <si>
@@ -437,13 +439,16 @@
   </si>
   <si>
     <t>Borroni Albert</t>
+  </si>
+  <si>
+    <t>Computer and Information Security</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,12 +798,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1">
@@ -876,7 +886,7 @@
         <v>99</v>
       </c>
       <c r="M2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -902,7 +912,7 @@
         <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -928,7 +938,7 @@
         <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -954,7 +964,7 @@
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -980,7 +990,7 @@
         <v>100</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1006,7 +1016,7 @@
         <v>100</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1047,7 +1057,7 @@
         <v>99</v>
       </c>
       <c r="M8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1073,7 +1083,7 @@
         <v>99</v>
       </c>
       <c r="I9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1099,7 +1109,7 @@
         <v>99</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1125,7 +1135,7 @@
         <v>100</v>
       </c>
       <c r="I11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1151,7 +1161,7 @@
         <v>100</v>
       </c>
       <c r="I12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1177,7 +1187,7 @@
         <v>100</v>
       </c>
       <c r="I13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1218,7 +1228,7 @@
         <v>99</v>
       </c>
       <c r="M14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1244,7 +1254,7 @@
         <v>99</v>
       </c>
       <c r="I15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1270,7 +1280,7 @@
         <v>99</v>
       </c>
       <c r="I16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1296,7 +1306,7 @@
         <v>100</v>
       </c>
       <c r="I17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1322,7 +1332,7 @@
         <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1348,7 +1358,7 @@
         <v>100</v>
       </c>
       <c r="I19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1389,7 +1399,7 @@
         <v>101</v>
       </c>
       <c r="M20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1415,7 +1425,7 @@
         <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1441,7 +1451,7 @@
         <v>101</v>
       </c>
       <c r="I22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1467,7 +1477,7 @@
         <v>102</v>
       </c>
       <c r="I23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1493,7 +1503,7 @@
         <v>102</v>
       </c>
       <c r="I24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1519,7 +1529,7 @@
         <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1560,7 +1570,7 @@
         <v>101</v>
       </c>
       <c r="M26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1586,7 +1596,7 @@
         <v>101</v>
       </c>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1612,7 +1622,7 @@
         <v>101</v>
       </c>
       <c r="I28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1638,7 +1648,7 @@
         <v>102</v>
       </c>
       <c r="I29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1664,7 +1674,7 @@
         <v>102</v>
       </c>
       <c r="I30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1690,7 +1700,7 @@
         <v>102</v>
       </c>
       <c r="I31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1731,7 +1741,7 @@
         <v>101</v>
       </c>
       <c r="M32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1757,7 +1767,7 @@
         <v>101</v>
       </c>
       <c r="I33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1783,7 +1793,7 @@
         <v>101</v>
       </c>
       <c r="I34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1809,7 +1819,7 @@
         <v>102</v>
       </c>
       <c r="I35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1835,7 +1845,7 @@
         <v>102</v>
       </c>
       <c r="I36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1861,7 +1871,7 @@
         <v>102</v>
       </c>
       <c r="I37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -1902,7 +1912,7 @@
         <v>100</v>
       </c>
       <c r="M38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -1957,10 +1967,10 @@
         <v>95</v>
       </c>
       <c r="L40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2006,19 +2016,19 @@
         <v>104</v>
       </c>
       <c r="I42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K42" t="s">
         <v>95</v>
       </c>
       <c r="L42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2047,7 +2057,7 @@
         <v>105</v>
       </c>
       <c r="I43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J43" t="s">
         <v>93</v>
@@ -2056,10 +2066,10 @@
         <v>95</v>
       </c>
       <c r="L43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2097,10 +2107,10 @@
         <v>95</v>
       </c>
       <c r="L44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2129,19 +2139,19 @@
         <v>107</v>
       </c>
       <c r="I45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K45" t="s">
         <v>95</v>
       </c>
       <c r="L45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2173,16 +2183,16 @@
         <v>83</v>
       </c>
       <c r="J46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K46" t="s">
         <v>95</v>
       </c>
       <c r="L46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2208,22 +2218,22 @@
         <v>97</v>
       </c>
       <c r="H47" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="I47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K47" t="s">
         <v>95</v>
       </c>
       <c r="L47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2249,7 +2259,7 @@
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I48" t="s">
         <v>39</v>
@@ -2261,10 +2271,10 @@
         <v>95</v>
       </c>
       <c r="L48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2290,22 +2300,22 @@
         <v>20</v>
       </c>
       <c r="H49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K49" t="s">
         <v>95</v>
       </c>
       <c r="L49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2328,19 +2338,19 @@
         <v>88</v>
       </c>
       <c r="H50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -2363,19 +2373,19 @@
         <v>88</v>
       </c>
       <c r="H51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2398,19 +2408,19 @@
         <v>88</v>
       </c>
       <c r="H52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -2433,19 +2443,19 @@
         <v>88</v>
       </c>
       <c r="H53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2468,19 +2478,19 @@
         <v>88</v>
       </c>
       <c r="H54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2503,19 +2513,19 @@
         <v>88</v>
       </c>
       <c r="H55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2538,16 +2548,16 @@
         <v>88</v>
       </c>
       <c r="H56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2570,16 +2580,16 @@
         <v>88</v>
       </c>
       <c r="H57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -2602,16 +2612,16 @@
         <v>88</v>
       </c>
       <c r="H58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -2634,16 +2644,16 @@
         <v>88</v>
       </c>
       <c r="H59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -2666,16 +2676,16 @@
         <v>88</v>
       </c>
       <c r="H60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -2698,16 +2708,16 @@
         <v>88</v>
       </c>
       <c r="H61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -2730,16 +2740,16 @@
         <v>88</v>
       </c>
       <c r="H62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -2762,16 +2772,16 @@
         <v>88</v>
       </c>
       <c r="H63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -2794,16 +2804,16 @@
         <v>88</v>
       </c>
       <c r="H64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -2826,16 +2836,16 @@
         <v>88</v>
       </c>
       <c r="H65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -2858,16 +2868,16 @@
         <v>88</v>
       </c>
       <c r="H66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -2890,16 +2900,16 @@
         <v>88</v>
       </c>
       <c r="H67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -2922,19 +2932,19 @@
         <v>88</v>
       </c>
       <c r="H68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -2957,19 +2967,19 @@
         <v>88</v>
       </c>
       <c r="H69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -2992,19 +3002,19 @@
         <v>88</v>
       </c>
       <c r="H70" t="s">
+        <v>113</v>
+      </c>
+      <c r="J70" t="s">
+        <v>120</v>
+      </c>
+      <c r="K70" t="s">
+        <v>121</v>
+      </c>
+      <c r="L70" t="s">
+        <v>121</v>
+      </c>
+      <c r="M70" t="s">
         <v>114</v>
-      </c>
-      <c r="J70" t="s">
-        <v>121</v>
-      </c>
-      <c r="K70" t="s">
-        <v>122</v>
-      </c>
-      <c r="L70" t="s">
-        <v>122</v>
-      </c>
-      <c r="M70" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3027,19 +3037,19 @@
         <v>88</v>
       </c>
       <c r="H71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -3062,19 +3072,19 @@
         <v>88</v>
       </c>
       <c r="H72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -3097,19 +3107,19 @@
         <v>88</v>
       </c>
       <c r="H73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -3132,19 +3142,19 @@
         <v>88</v>
       </c>
       <c r="H74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -3167,19 +3177,19 @@
         <v>88</v>
       </c>
       <c r="H75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J75" t="s">
+        <v>127</v>
+      </c>
+      <c r="K75" t="s">
+        <v>121</v>
+      </c>
+      <c r="L75" t="s">
+        <v>121</v>
+      </c>
+      <c r="M75" t="s">
         <v>128</v>
-      </c>
-      <c r="K75" t="s">
-        <v>122</v>
-      </c>
-      <c r="L75" t="s">
-        <v>122</v>
-      </c>
-      <c r="M75" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -3202,19 +3212,19 @@
         <v>88</v>
       </c>
       <c r="H76" t="s">
+        <v>113</v>
+      </c>
+      <c r="J76" t="s">
+        <v>127</v>
+      </c>
+      <c r="K76" t="s">
+        <v>121</v>
+      </c>
+      <c r="L76" t="s">
+        <v>121</v>
+      </c>
+      <c r="M76" t="s">
         <v>114</v>
-      </c>
-      <c r="J76" t="s">
-        <v>128</v>
-      </c>
-      <c r="K76" t="s">
-        <v>122</v>
-      </c>
-      <c r="L76" t="s">
-        <v>122</v>
-      </c>
-      <c r="M76" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -3237,19 +3247,19 @@
         <v>88</v>
       </c>
       <c r="H77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -3272,19 +3282,19 @@
         <v>88</v>
       </c>
       <c r="H78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3307,19 +3317,19 @@
         <v>88</v>
       </c>
       <c r="H79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3342,22 +3352,27 @@
         <v>88</v>
       </c>
       <c r="H80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K80" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L80" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>